<commit_message>
json to dataframe, csv and excel method added
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,22 +466,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>132</t>
+          <t>0ecb9182-4496-4e28-ab35-a9760614a8c7.jpg</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>gupta/Chandragupta II</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>archer type</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>isadksahd</t>
+          <t xml:space="preserve">Lorem Ipsum is simply dummy text of the printing and typesetting industry. Lorem Ipsum has been the industry's standard dummy text ever since the 1500s, when an unknown printer took a galley of type and scrambled it to make a type specimen book. </t>
         </is>
       </c>
     </row>
@@ -491,22 +491,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>132</t>
+          <t>0ecb9182-4496-4e28-ab35-a9760614a8c7.jpg</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>gupta/Skandagupta</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>archer type</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>isadksahd</t>
+          <t xml:space="preserve">Lorem Ipsum is simply dummy text of the printing and typesetting industry. Lorem Ipsum has been the industry's standard dummy text ever since the 1500s, when an unknown printer took a galley of type and scrambled it to make a type specimen book. </t>
         </is>
       </c>
     </row>
@@ -516,47 +516,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>jhagsdg</t>
+          <t>0ecb9182-4496-4e28-ab35-a9760614a8c7.jpg</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>asdjh</t>
+          <t>gupta/Skandagupta</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>archer type</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>isadksahd</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>uiy6euwd</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>isadksahd</t>
+          <t xml:space="preserve">Lorem Ipsum is simply dummy text of the printing and typesetting industry. Lorem Ipsum has been the industry's standard dummy text ever since the 1500s, when an unknown printer took a galley of type and scrambled it to make a type specimen book. </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
privide some real data for testing
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,12 +466,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0ecb9182-4496-4e28-ab35-a9760614a8c7.jpg</t>
+          <t>Skanda-4865A-654.50-obverse.jpg</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>gupta/Chandragupta II</t>
+          <t>Gupta/Skandagupta</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -481,7 +481,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Lorem Ipsum is simply dummy text of the printing and typesetting industry. Lorem Ipsum has been the industry's standard dummy text ever since the 1500s, when an unknown printer took a galley of type and scrambled it to make a type specimen book. </t>
+          <t>King standing and holding an Indian long bow in his left hand and an arrow in his right Garuda standard at left;Brāhmī legend under arm: skanda</t>
         </is>
       </c>
     </row>
@@ -491,12 +491,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0ecb9182-4496-4e28-ab35-a9760614a8c7.jpg</t>
+          <t>Skanda-4865A-654.50-reverse.jpg</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>gupta/Skandagupta</t>
+          <t>Gupta/Skandagupta</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -506,7 +506,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Lorem Ipsum is simply dummy text of the printing and typesetting industry. Lorem Ipsum has been the industry's standard dummy text ever since the 1500s, when an unknown printer took a galley of type and scrambled it to make a type specimen book. </t>
+          <t>Lakshmi seated facing, holding long-stemmed lotus and diadem;Brāhmī legend at right: sri skandaguptah;circular Brāhmī legend around</t>
         </is>
       </c>
     </row>
@@ -516,12 +516,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>0ecb9182-4496-4e28-ab35-a9760614a8c7.jpg</t>
+          <t>Skanda-4865-148.06-obverse.jpg</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>gupta/Skandagupta</t>
+          <t>Gupta/Skandagupta</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -531,7 +531,82 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Lorem Ipsum is simply dummy text of the printing and typesetting industry. Lorem Ipsum has been the industry's standard dummy text ever since the 1500s, when an unknown printer took a galley of type and scrambled it to make a type specimen book. </t>
+          <t>King standing and holding an Indian long bow in his left hand and an arrow in his right Garuda standard at left;Brāhmī legend under arm: skanda;circular Brāhmī legend around</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Skanda-4865-148.06-reverse.jpg</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Gupta/Skandagupta</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>archer type</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Lakshmi seated facing, holding long-stemmed lotus and diadem;Brāhmī legend at right: kramadityah</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Skanda-4866-421.04-obverse.jpg</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Gupta/Skandagupta</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>archer type;King and Lakshmi type</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>King standing at left, facing right and holding an Indian long bow in his left hand and an arrow in his right hand, Lakshmi standing at right, facing left and offering an indistinct object to the king Garuda standard between the two figures,</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Skanda-4866-421.04-reverse.jpg</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Gupta/Skandagupta</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>archer type</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Lakshmi seated facing, holding long-stemmed lotus and diadem;Brāhmī legend at right: sri skandaguptah;circular Brāhmī legend around</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added label of the coin
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,11 @@
           <t>details</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -484,6 +489,11 @@
           <t>King standing and holding an Indian long bow in his left hand and an arrow in his right Garuda standard at left;Brāhmī legend under arm: skanda</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -509,6 +519,11 @@
           <t>Lakshmi seated facing, holding long-stemmed lotus and diadem;Brāhmī legend at right: sri skandaguptah;circular Brāhmī legend around</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -534,6 +549,11 @@
           <t>King standing and holding an Indian long bow in his left hand and an arrow in his right Garuda standard at left;Brāhmī legend under arm: skanda;circular Brāhmī legend around</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -559,6 +579,11 @@
           <t>Lakshmi seated facing, holding long-stemmed lotus and diadem;Brāhmī legend at right: kramadityah</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -584,6 +609,11 @@
           <t>King standing at left, facing right and holding an Indian long bow in his left hand and an arrow in his right hand, Lakshmi standing at right, facing left and offering an indistinct object to the king Garuda standard between the two figures,</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>real</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -607,6 +637,11 @@
       <c r="E7" t="inlineStr">
         <is>
           <t>Lakshmi seated facing, holding long-stemmed lotus and diadem;Brāhmī legend at right: sri skandaguptah;circular Brāhmī legend around</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>real</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
data pulling system updated
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -474,25 +474,19 @@
           <t>Skanda-4865A-654.50-obverse.jpg</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Gupta/Skandagupta</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>archer type</t>
-        </is>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
           <t>King standing and holding an Indian long bow in his left hand and an arrow in his right Garuda standard at left;Brāhmī legend under arm: skanda</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>real</t>
-        </is>
+      <c r="F2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -504,25 +498,19 @@
           <t>Skanda-4865A-654.50-reverse.jpg</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Gupta/Skandagupta</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>archer type</t>
-        </is>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>Lakshmi seated facing, holding long-stemmed lotus and diadem;Brāhmī legend at right: sri skandaguptah;circular Brāhmī legend around</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>real</t>
-        </is>
+      <c r="F3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -534,25 +522,19 @@
           <t>Skanda-4865-148.06-obverse.jpg</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Gupta/Skandagupta</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>archer type</t>
-        </is>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
           <t>King standing and holding an Indian long bow in his left hand and an arrow in his right Garuda standard at left;Brāhmī legend under arm: skanda;circular Brāhmī legend around</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>real</t>
-        </is>
+      <c r="F4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -564,25 +546,19 @@
           <t>Skanda-4865-148.06-reverse.jpg</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Gupta/Skandagupta</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>archer type</t>
-        </is>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>Lakshmi seated facing, holding long-stemmed lotus and diadem;Brāhmī legend at right: kramadityah</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>real</t>
-        </is>
+      <c r="F5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -594,25 +570,19 @@
           <t>Skanda-4866-421.04-obverse.jpg</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Gupta/Skandagupta</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>archer type;King and Lakshmi type</t>
-        </is>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
           <t>King standing at left, facing right and holding an Indian long bow in his left hand and an arrow in his right hand, Lakshmi standing at right, facing left and offering an indistinct object to the king Garuda standard between the two figures,</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>real</t>
-        </is>
+      <c r="F6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -624,25 +594,19 @@
           <t>Skanda-4866-421.04-reverse.jpg</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Gupta/Skandagupta</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>archer type</t>
-        </is>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
           <t>Lakshmi seated facing, holding long-stemmed lotus and diadem;Brāhmī legend at right: sri skandaguptah;circular Brāhmī legend around</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>fake</t>
-        </is>
+      <c r="F7" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data creation system change and added some coin data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,7 +482,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>King standing and holding an Indian long bow in his left hand and an arrow in his right Garuda standard at left;Brāhmī legend under arm: skanda</t>
+          <t>King standing and holding an Indian long bow in his left hand and an arrow in his right Garuda standard at left;Brahmi legend under arm: skanda</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -506,7 +506,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Lakshmi seated facing, holding long-stemmed lotus and diadem;Brāhmī legend at right: sri skandaguptah;circular Brāhmī legend around</t>
+          <t>Lakshmi seated facing and holding long-stemmed lotus and diadem;Brahmi legend at right: sri skandaguptah;circular Brahmi legend around</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -530,7 +530,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>King standing and holding an Indian long bow in his left hand and an arrow in his right Garuda standard at left;Brāhmī legend under arm: skanda;circular Brāhmī legend around</t>
+          <t>King standing and holding an Indian long bow in his left hand and an arrow in his right Garuda standard at left;Brahmi legend under arm: skanda;circular Brahmi legend around</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -554,7 +554,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Lakshmi seated facing, holding long-stemmed lotus and diadem;Brāhmī legend at right: kramadityah</t>
+          <t>Lakshmi seated facing and holding long-stemmed lotus and diadem;Brahmi legend at right: kramadityah</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -578,7 +578,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>King standing at left, facing right and holding an Indian long bow in his left hand and an arrow in his right hand, Lakshmi standing at right, facing left and offering an indistinct object to the king Garuda standard between the two figures,</t>
+          <t>King standing at left and facing right and holding an Indian long bow in his left hand and an arrow in his right hand, Lakshmi standing at right, facing left and offering an indistinct object to the king Garuda standard between the two figures,</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -602,10 +602,130 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Lakshmi seated facing, holding long-stemmed lotus and diadem;Brāhmī legend at right: sri skandaguptah;circular Brāhmī legend around</t>
+          <t>Lakshmi seated facing and holding long-stemmed lotus and diadem;Brahmi legend at right: sri skandaguptah;circular Brahmi legend around</t>
         </is>
       </c>
       <c r="F7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Kumara-4829v-625.13-obverse.jpg</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>King standing and holding an Indian long bow in his left hand and an arrow in his right Garuda standard at left;Brahmi legend in right field: Kumara</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Kumara-4829v-625.13-reverse.jpg</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Lakshmi seated facing and holding long-stemmed lotus and scattering coins with her right hand;Brahmi legend at right: Sri Mahendra;circular Brahmi legend around</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Kumara-4830-280.60-obverse.jpg</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>King standing and holding an Indian long bow in his left hand and an arrow in his right Garuda standard at left;Brahmi legend under arm: Ku;circular Brahmi legend around</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Kumara-4830-280.60-reverse.jpg</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Lakshmi seated facing and holding long-stemmed lotus and diadem;Brahmi legend at right: Sri Mahendra;</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Kumara-4834-486.22-obverse.jpg</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>King standing and holding an Indian long bow in his left hand and an arrow in his right Garuda standard at left, Brāhmī legend under arm: Ku</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>